<commit_message>
fix calculations with #N/A values
</commit_message>
<xml_diff>
--- a/tests/ast/basic_evaluation.xlsx
+++ b/tests/ast/basic_evaluation.xlsx
@@ -1,14 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\skybonds\oxford\koala\tests\ast\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="680" windowWidth="25520" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="2565" yWindow="675" windowWidth="25515" windowHeight="15600" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="EmptyRange">Sheet1!$A$12:$G$12</definedName>
@@ -21,7 +27,7 @@
     <definedName name="Liste5">Sheet1!$C$31:$F$31</definedName>
     <definedName name="NOP">Sheet1!$N$7:$P$7</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" calcMode="autoNoTable"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -74,7 +80,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -134,24 +140,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="6" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -479,13 +494,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -536,7 +551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -580,7 +595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -620,7 +635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
@@ -631,7 +646,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -648,12 +663,12 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -665,7 +680,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>8</v>
       </c>
@@ -684,15 +699,15 @@
       <c r="O9" s="3"/>
       <c r="P9" s="4"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P11" s="3"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ref="A13:G13" si="2">EmptyRange</f>
         <v>0</v>
@@ -722,7 +737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -755,7 +770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>30</v>
       </c>
@@ -792,7 +807,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -837,7 +852,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6</v>
       </c>
@@ -867,7 +882,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>11</v>
       </c>
@@ -897,7 +912,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I25">
         <v>40</v>
       </c>
@@ -912,7 +927,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B26" t="e">
         <f>A22:B24+A22:C22</f>
         <v>#VALUE!</v>
@@ -926,7 +941,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C30">
         <v>1</v>
       </c>
@@ -940,7 +955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
@@ -964,7 +979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C32">
         <f>Liste5 +10</f>
         <v>12</v>
@@ -993,12 +1008,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K33" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -1006,7 +1021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <f>2%+A36</f>
         <v>1.02</v>
@@ -1016,13 +1031,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="array" ref="A39">IFERROR(MATCH(TRUE,Liste&gt;2,0),"Rien")</f>
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>CHOOSE(A1, J22,J23,J24,J25)</f>
         <v>Paul</v>
@@ -1046,14 +1061,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1062,47 +1077,47 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
@@ -1111,47 +1126,47 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
@@ -1164,4 +1179,68 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5">
+        <v>36892</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>SUM(A1:A2)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>AVERAGE(A1:A2)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>MAX(A1:A2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>MIN(A1:A2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f>ROUND(XNPV(1,A1:A2,B1:B2), 3)</f>
+        <v>1.998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>